<commit_message>
manual hidden vector assignment
</commit_message>
<xml_diff>
--- a/w2/w2.xlsx
+++ b/w2/w2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
   <si>
     <r>
       <t xml:space="preserve">Determine the rest of the entries in </t>
@@ -67,12 +68,42 @@
       <t xml:space="preserve"> = (0.6, 0.82) and the five sequences of coin flips, reproduced below.</t>
     </r>
   </si>
+  <si>
+    <t>θa</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>θb</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>HVb</t>
+  </si>
+  <si>
+    <t>HVa</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +126,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -124,6 +161,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,15 +185,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4448174</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57177</xdr:rowOff>
+      <xdr:colOff>4314825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -170,7 +209,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -184,8 +223,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="1085849"/>
-          <a:ext cx="4448174" cy="1819303"/>
+          <a:off x="1771650" y="1352550"/>
+          <a:ext cx="2543175" cy="1123950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -204,6 +243,184 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8564916-2B17-40F0-B3C2-6E13F96B12E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="361950" y="1190625"/>
+          <a:ext cx="2543175" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2543175" cy="1095375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{177462B9-FD2F-407A-9924-C3114B852AD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="361950" y="1190625"/>
+          <a:ext cx="2543175" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2543175" cy="1095375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA6ABE3-10F6-4074-AE38-05D857C7B797}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="361950" y="2905125"/>
+          <a:ext cx="2543175" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -504,20 +721,911 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <f>$A$12-B7</f>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ref="C8:C11" si="0">$A$12-B8</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F5:Q33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I6" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="O6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f>G8/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f>$H$5-G8</f>
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <f>$I$6^G8*(1-$I$6)^H8</f>
+        <v>5.3084160000000031E-4</v>
+      </c>
+      <c r="J8">
+        <f>$J$6^G8*(1-$J$6)^H8</f>
+        <v>1.5377666576394263E-5</v>
+      </c>
+      <c r="L8">
+        <f>IF(I8&gt;J8,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f>IF(J8&gt;I8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>I8/SUM($I8:$J8)</f>
+        <v>0.97184708135108688</v>
+      </c>
+      <c r="P8">
+        <f>J8/SUM($I8:$J8)</f>
+        <v>2.815291864891319E-2</v>
+      </c>
+      <c r="Q8">
+        <f>SUM(O8:P8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" ref="F9:F12" si="0">G9/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H12" si="1">$H$5-G9</f>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I12" si="2">$I$6^G9*(1-$I$6)^H9</f>
+        <v>4.0310783999999997E-3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9:J12" si="3">$J$6^G9*(1-$J$6)^H9</f>
+        <v>3.0171519073747433E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L12" si="4">IF(I9&gt;J9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M12" si="5">IF(J9&gt;I9,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:O12" si="6">I9/SUM($I9:$J9)</f>
+        <v>0.11785883815093567</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P12" si="7">J9/SUM($I9:$J9)</f>
+        <v>0.88214116184906433</v>
+      </c>
+      <c r="Q9">
+        <f>SUM(O9:P9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2.6873856000000002E-3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>6.6230163820421217E-3</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>0.28864334807277087</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="7"/>
+        <v>0.71135665192722908</v>
+      </c>
+      <c r="Q10">
+        <f>SUM(O10:P10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>3.5389440000000024E-4</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>3.3755853460377657E-6</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>0.99055172422959548</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="7"/>
+        <v>9.4482757704045673E-3</v>
+      </c>
+      <c r="Q11">
+        <f>SUM(O11:P11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>1.7915904000000002E-3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>1.4538328643507101E-3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>0.55203597622525558</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="7"/>
+        <v>0.44796402377474437</v>
+      </c>
+      <c r="Q12">
+        <f>SUM(O12:P12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f>SUMPRODUCT(F8:F12,L8:L12)/SUM(L8:L12)</f>
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="J15">
+        <f>SUMPRODUCT(F8:F12,M8:M12)/SUM(M8:M12)</f>
+        <v>0.85000000000000009</v>
+      </c>
+    </row>
+    <row r="16" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f>G17/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <f>$H$5-G17</f>
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <f>$I$15^G17*(1-$I$15)^H17</f>
+        <v>1.0914893221832722E-3</v>
+      </c>
+      <c r="J17">
+        <f>$J$15^G17*(1-$J$15)^H17</f>
+        <v>5.9459774414062329E-6</v>
+      </c>
+      <c r="L17">
+        <f>IF(I17&gt;J17,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f>IF(J17&gt;I17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>I17/SUM($I17:$J17)</f>
+        <v>0.9945819334921705</v>
+      </c>
+      <c r="P17">
+        <f>J17/SUM($I17:$J17)</f>
+        <v>5.4180665078294365E-3</v>
+      </c>
+      <c r="Q17">
+        <f>SUM(O17:P17)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" ref="F18:F21" si="8">G18/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="G18">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H21" si="9">$H$5-G18</f>
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ref="I18:I21" si="10">$I$15^G18*(1-$I$15)^H18</f>
+        <v>5.5983462640180146E-4</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:J21" si="11">$J$15^G18*(1-$J$15)^H18</f>
+        <v>3.4742541942480477E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L21" si="12">IF(I18&gt;J18,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M21" si="13">IF(J18&gt;I18,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18:O21" si="14">I18/SUM($I18:$J18)</f>
+        <v>1.5858270201991861E-2</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18:P21" si="15">J18/SUM($I18:$J18)</f>
+        <v>0.98414172979800818</v>
+      </c>
+      <c r="Q18">
+        <f>SUM(O18:P18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="10"/>
+        <v>6.3981100160205909E-4</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="11"/>
+        <v>6.1310368133789045E-3</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="14"/>
+        <v>9.4494961205069991E-2</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="15"/>
+        <v>0.90550503879492994</v>
+      </c>
+      <c r="Q19">
+        <f>SUM(O19:P19)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="8"/>
+        <v>0.3</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="10"/>
+        <v>1.2474163682094544E-3</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="11"/>
+        <v>1.0492901367187463E-6</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="14"/>
+        <v>0.99915953624378517</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="15"/>
+        <v>8.404637562147506E-4</v>
+      </c>
+      <c r="Q20">
+        <f>SUM(O20:P20)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>0.7</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="10"/>
+        <v>7.3121257325949626E-4</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="11"/>
+        <v>1.0819476729492176E-3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="14"/>
+        <v>0.40328072203681326</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="15"/>
+        <v>0.59671927796318669</v>
+      </c>
+      <c r="Q21">
+        <f>SUM(O21:P21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f>SUMPRODUCT(F17:F21,L17:L21)/SUM(L17:L21)</f>
+        <v>0.35</v>
+      </c>
+      <c r="J24">
+        <f>SUMPRODUCT(F17:F21,M17:M21)/SUM(M17:M21)</f>
+        <v>0.80000000000000016</v>
+      </c>
+    </row>
+    <row r="25" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f>G26/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <f>$H$5-G26</f>
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <f>$I$24^G26*(1-$I$24)^H26</f>
+        <v>1.1317547274414064E-3</v>
+      </c>
+      <c r="J26">
+        <f>$J$24^G26*(1-$J$24)^H26</f>
+        <v>2.6214399999999896E-5</v>
+      </c>
+      <c r="L26">
+        <f>IF(I26&gt;J26,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f>IF(J26&gt;I26,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>I26/SUM($I26:$J26)</f>
+        <v>0.97736174533605924</v>
+      </c>
+      <c r="P26">
+        <f>J26/SUM($I26:$J26)</f>
+        <v>2.2638254663940819E-2</v>
+      </c>
+      <c r="Q26">
+        <f>SUM(O26:P26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" ref="F27:F30" si="16">G27/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H30" si="17">$H$5-G27</f>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I30" si="18">$I$24^G27*(1-$I$24)^H27</f>
+        <v>5.1230165136718714E-5</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27:J30" si="19">$J$24^G27*(1-$J$24)^H27</f>
+        <v>2.6843545600000025E-2</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ref="L27:L30" si="20">IF(I27&gt;J27,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M30" si="21">IF(J27&gt;I27,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ref="O27:O30" si="22">I27/SUM($I27:$J27)</f>
+        <v>1.904837042855272E-3</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ref="P27:P30" si="23">J27/SUM($I27:$J27)</f>
+        <v>0.99809516295714473</v>
+      </c>
+      <c r="Q27">
+        <f>SUM(O27:P27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="16"/>
+        <v>0.8</v>
+      </c>
+      <c r="G28">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="18"/>
+        <v>9.5141735253906196E-5</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="19"/>
+        <v>6.7108863999999994E-3</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="22"/>
+        <v>1.3979039369686185E-2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="23"/>
+        <v>0.98602096063031375</v>
+      </c>
+      <c r="Q28">
+        <f>SUM(O28:P28)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="29" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="16"/>
+        <v>0.3</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="18"/>
+        <v>2.1018302081054693E-3</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="19"/>
+        <v>6.5535999999999672E-6</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="22"/>
+        <v>0.99689164753836312</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="23"/>
+        <v>3.1083524616368763E-3</v>
+      </c>
+      <c r="Q29">
+        <f>SUM(O29:P29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="16"/>
+        <v>0.7</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="18"/>
+        <v>1.7669179404296867E-4</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="19"/>
+        <v>1.6777215999999979E-3</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="22"/>
+        <v>9.5281771912651941E-2</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="23"/>
+        <v>0.90471822808734814</v>
+      </c>
+      <c r="Q30">
+        <f>SUM(O30:P30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f>SUMPRODUCT(F26:F30,L26:L30)/SUM(L26:L30)</f>
+        <v>0.35</v>
+      </c>
+      <c r="J33">
+        <f>SUMPRODUCT(F26:F30,M26:M30)/SUM(M26:M30)</f>
+        <v>0.80000000000000016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some of week's 2 work done
</commit_message>
<xml_diff>
--- a/w2/w2.xlsx
+++ b/w2/w2.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EM_soft_assignments" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,107 +22,419 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="43">
+  <si>
+    <t>θa</t>
+  </si>
+  <si>
+    <t>θb</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>HVb</t>
+  </si>
+  <si>
+    <t>HVa</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
+  <si>
+    <t>ones</t>
+  </si>
   <si>
     <r>
-      <t xml:space="preserve">Determine the rest of the entries in </t>
+      <t>Exercise Break:</t>
     </r>
     <r>
       <rPr>
-        <i/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">HiddenVector </t>
+      <t xml:space="preserve"> Compute </t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <i/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">for </t>
+      <t>HiddenMatrix</t>
     </r>
     <r>
       <rPr>
-        <i/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Parameters</t>
+      <t xml:space="preserve"> using the Newtonian inverse-square law for the three centers and eight data points shown in the figure below.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HiddenMatrix</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <i/>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>=1/</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>Data</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Size1"/>
+      </rPr>
+      <t>∑</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>all centers </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5.5"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>1/</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>Data</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.4"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = (0.6, 0.82) and the five sequences of coin flips, reproduced below.</t>
+      <t>.</t>
     </r>
   </si>
   <si>
-    <t>θa</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>θb</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>HVb</t>
-  </si>
-  <si>
-    <t>HVa</t>
-  </si>
-  <si>
-    <t>soft</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>center1</t>
+  </si>
+  <si>
+    <t>center2</t>
+  </si>
+  <si>
+    <t>center3</t>
+  </si>
+  <si>
+    <t>item1</t>
+  </si>
+  <si>
+    <t>item2</t>
+  </si>
+  <si>
+    <t>item3</t>
+  </si>
+  <si>
+    <t>item4</t>
+  </si>
+  <si>
+    <t>item5</t>
+  </si>
+  <si>
+    <t>item6</t>
+  </si>
+  <si>
+    <t>item7</t>
+  </si>
+  <si>
+    <t>item8</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>distances</t>
+  </si>
+  <si>
+    <t>distances2</t>
+  </si>
+  <si>
+    <t>HM</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>partition function</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>p7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,6 +445,68 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13.4"/>
+      <color theme="1"/>
+      <name val="MathJax_Main"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7.75"/>
+      <color theme="1"/>
+      <name val="MathJax_Math"/>
+    </font>
+    <font>
+      <sz val="7.75"/>
+      <color theme="1"/>
+      <name val="MathJax_Main"/>
+    </font>
+    <font>
+      <sz val="13.4"/>
+      <color theme="1"/>
+      <name val="MathJax_Main"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13.4"/>
+      <color theme="1"/>
+      <name val="MathJax_Math"/>
+    </font>
+    <font>
+      <sz val="13.4"/>
+      <color theme="1"/>
+      <name val="MathJax_Size1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="5.5"/>
+      <color theme="1"/>
+      <name val="MathJax_Math"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,16 +529,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,22 +564,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1771650</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4314825</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AE76F57-AEF9-4EEE-B56F-D0DA2BF48F53}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50CCE00F-B308-404A-8F04-A7185BDB2D3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -223,8 +602,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1771650" y="1352550"/>
-          <a:ext cx="2543175" cy="1123950"/>
+          <a:off x="361950" y="1190625"/>
+          <a:ext cx="2543175" cy="1095375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -243,6 +622,174 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2543175" cy="1095375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F51B5E0-28EE-4419-9790-3F2DF6B37BC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="361950" y="2905125"/>
+          <a:ext cx="2543175" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2543175" cy="1095375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D64E824D-D936-4361-87C1-045343478C2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="361950" y="4619625"/>
+          <a:ext cx="2543175" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2543175" cy="1095375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A965A436-DFFB-4B13-8B89-4F605CD144FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="361950" y="4619625"/>
+          <a:ext cx="2543175" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -421,6 +968,72 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3390900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>64580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="http://bioinformaticsalgorithms.com/images/Clustering/maxdistance_vs_error_distortion_1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FCFF8C4-11A4-42F9-91FA-054D325CB3C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="133350" y="676275"/>
+          <a:ext cx="3257550" cy="3007805"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -721,125 +1334,1065 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="F5:S42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
+    <row r="5" spans="6:19">
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="6:19">
+      <c r="I6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="O6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="6:19">
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="6:19">
+      <c r="F8">
+        <f>G8/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f>$H$5-G8</f>
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <f>$I$6^G8*(1-$I$6)^H8</f>
+        <v>5.3084160000000031E-4</v>
+      </c>
+      <c r="J8">
+        <f>$J$6^G8*(1-$J$6)^H8</f>
+        <v>1.5377666576394263E-5</v>
+      </c>
+      <c r="L8">
+        <f>IF(I8&gt;J8,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f>IF(J8&gt;I8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>I8/SUM($I8:$J8)</f>
+        <v>0.97184708135108688</v>
+      </c>
+      <c r="P8">
+        <f>J8/SUM($I8:$J8)</f>
+        <v>2.815291864891319E-2</v>
+      </c>
+      <c r="Q8">
+        <f>SUM(O8:P8)</f>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="6:19">
+      <c r="F9">
+        <f t="shared" ref="F9:F12" si="0">G9/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H12" si="1">$H$5-G9</f>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I12" si="2">$I$6^G9*(1-$I$6)^H9</f>
+        <v>4.0310783999999997E-3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9:J12" si="3">$J$6^G9*(1-$J$6)^H9</f>
+        <v>3.0171519073747433E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L12" si="4">IF(I9&gt;J9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M12" si="5">IF(J9&gt;I9,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:O12" si="6">I9/SUM($I9:$J9)</f>
+        <v>0.11785883815093567</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P12" si="7">J9/SUM($I9:$J9)</f>
+        <v>0.88214116184906433</v>
+      </c>
+      <c r="Q9">
+        <f>SUM(O9:P9)</f>
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="6:19">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2.6873856000000002E-3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>6.6230163820421217E-3</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>0.28864334807277087</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="7"/>
+        <v>0.71135665192722908</v>
+      </c>
+      <c r="Q10">
+        <f>SUM(O10:P10)</f>
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="6:19">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>3.5389440000000024E-4</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>3.3755853460377657E-6</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>0.99055172422959548</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="7"/>
+        <v>9.4482757704045673E-3</v>
+      </c>
+      <c r="Q11">
+        <f>SUM(O11:P11)</f>
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="6:19">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>1.7915904000000002E-3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>1.4538328643507101E-3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>0.55203597622525558</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="7"/>
+        <v>0.44796402377474437</v>
+      </c>
+      <c r="Q12">
+        <f>SUM(O12:P12)</f>
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="6:19">
+      <c r="L13">
+        <f>SUM(L8:L12)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="6:19">
+      <c r="I14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="6:19">
+      <c r="I15">
+        <f>SUMPRODUCT(F8:F12,O8:O12)/SUMPRODUCT(O8:O12,$S$8:$S$12)</f>
+        <v>0.48248804455089772</v>
+      </c>
+      <c r="J15">
+        <f>SUMPRODUCT(F8:F12,P8:P12)/SUMPRODUCT(P8:P12,$S$8:$S$12)</f>
+        <v>0.81319460162622714</v>
+      </c>
+    </row>
+    <row r="16" spans="6:19">
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="6:17">
+      <c r="F17">
+        <f>G17/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="G17">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
-        <f>$A$12-B7</f>
+      <c r="H17">
+        <f>$H$5-G17</f>
         <v>6</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="I17">
+        <f>$I$15^G17*(1-$I$15)^H17</f>
+        <v>1.0410427152127007E-3</v>
+      </c>
+      <c r="J17">
+        <f>$J$15^G17*(1-$J$15)^H17</f>
+        <v>1.8582942478529884E-5</v>
+      </c>
+      <c r="L17">
+        <f>IF(I17&gt;J17,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f>IF(J17&gt;I17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>I17/SUM($I17:$J17)</f>
+        <v>0.98246272884801655</v>
+      </c>
+      <c r="P17">
+        <f>J17/SUM($I17:$J17)</f>
+        <v>1.7537271151983426E-2</v>
+      </c>
+      <c r="Q17">
+        <f>SUM(O17:P17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="6:17">
+      <c r="F18">
+        <f t="shared" ref="F18:F21" si="8">G18/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="G18">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
-        <f t="shared" ref="C8:C11" si="0">$A$12-B8</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+      <c r="H18">
+        <f t="shared" ref="H18:H21" si="9">$H$5-G18</f>
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ref="I18:I21" si="10">$I$15^G18*(1-$I$15)^H18</f>
+        <v>7.3332990552663188E-4</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:J21" si="11">$J$15^G18*(1-$J$15)^H18</f>
+        <v>2.9049576458415854E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L21" si="12">IF(I18&gt;J18,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M21" si="13">IF(J18&gt;I18,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18:O21" si="14">I18/SUM($I18:$J18)</f>
+        <v>2.4622509857347517E-2</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18:P21" si="15">J18/SUM($I18:$J18)</f>
+        <v>0.97537749014265251</v>
+      </c>
+      <c r="Q18">
+        <f>SUM(O18:P18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="6:17">
+      <c r="F19">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+      <c r="G19">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
-        <f t="shared" si="0"/>
+      <c r="H19">
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="I19">
+        <f t="shared" si="10"/>
+        <v>7.8656248104891336E-4</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="11"/>
+        <v>6.6732092073060901E-3</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="14"/>
+        <v>0.10544055688416956</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="15"/>
+        <v>0.89455944311583047</v>
+      </c>
+      <c r="Q19">
+        <f>SUM(O19:P19)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="6:17">
+      <c r="F20">
+        <f t="shared" si="8"/>
+        <v>0.3</v>
+      </c>
+      <c r="G20">
         <v>3</v>
       </c>
-      <c r="C10" s="3">
-        <f t="shared" si="0"/>
+      <c r="H20">
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="I20">
+        <f t="shared" si="10"/>
+        <v>1.1166122297542953E-3</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="11"/>
+        <v>4.2688354862619414E-6</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="14"/>
+        <v>0.99619153573145081</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="15"/>
+        <v>3.8084642685491236E-3</v>
+      </c>
+      <c r="Q20">
+        <f>SUM(O20:P20)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="6:17">
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>0.7</v>
+      </c>
+      <c r="G21">
         <v>7</v>
       </c>
-      <c r="C11" s="3">
-        <f t="shared" si="0"/>
+      <c r="H21">
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="I21">
+        <f t="shared" si="10"/>
+        <v>8.4365922067438997E-4</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="11"/>
+        <v>1.5329559516374168E-3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="14"/>
+        <v>0.35498352047198989</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="15"/>
+        <v>0.64501647952801011</v>
+      </c>
+      <c r="Q21">
+        <f>SUM(O21:P21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="6:17">
+      <c r="I23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="6:17">
+      <c r="I24">
+        <f>SUMPRODUCT(F17:F21,O17:O21)/SUMPRODUCT(O17:O21,$S$8:$S$12)</f>
+        <v>0.42490699315468272</v>
+      </c>
+      <c r="J24">
+        <f>SUMPRODUCT(F17:F21,P17:P21)/SUMPRODUCT(P17:P21,$S$8:$S$12)</f>
+        <v>0.80950872080032232</v>
+      </c>
+    </row>
+    <row r="25" spans="6:17">
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" t="s">
+        <v>5</v>
+      </c>
+      <c r="L25" t="s">
+        <v>6</v>
+      </c>
+      <c r="M25" t="s">
+        <v>5</v>
+      </c>
+      <c r="O25" t="s">
+        <v>6</v>
+      </c>
+      <c r="P25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17">
+      <c r="F26">
+        <f>G26/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="G26">
         <v>4</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="H26">
+        <f>$H$5-G26</f>
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <f>$I$24^G26*(1-$I$24)^H26</f>
+        <v>1.1792449762298371E-3</v>
+      </c>
+      <c r="J26">
+        <f>$J$24^G26*(1-$J$24)^H26</f>
+        <v>2.0518079881527509E-5</v>
+      </c>
+      <c r="L26">
+        <f>IF(I26&gt;J26,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f>IF(J26&gt;I26,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>I26/SUM($I26:$J26)</f>
+        <v>0.98289822329749832</v>
+      </c>
+      <c r="P26">
+        <f>J26/SUM($I26:$J26)</f>
+        <v>1.7101776702501643E-2</v>
+      </c>
+      <c r="Q26">
+        <f>SUM(O26:P26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="6:17">
+      <c r="F27">
+        <f t="shared" ref="F27:F30" si="16">G27/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H30" si="17">$H$5-G27</f>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I30" si="18">$I$24^G27*(1-$I$24)^H27</f>
+        <v>2.5964681272762835E-4</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27:J30" si="19">$J$24^G27*(1-$J$24)^H27</f>
+        <v>2.8436024776346859E-2</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ref="L27:L30" si="20">IF(I27&gt;J27,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M30" si="21">IF(J27&gt;I27,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ref="O27:O30" si="22">I27/SUM($I27:$J27)</f>
+        <v>9.0482918973217412E-3</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ref="P27:P30" si="23">J27/SUM($I27:$J27)</f>
+        <v>0.9909517081026783</v>
+      </c>
+      <c r="Q27">
+        <f>SUM(O27:P27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="6:17">
+      <c r="F28">
+        <f t="shared" si="16"/>
+        <v>0.8</v>
+      </c>
+      <c r="G28">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="18"/>
+        <v>3.5142059004657537E-4</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="19"/>
+        <v>6.6914841011776844E-3</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="22"/>
+        <v>4.9897109992764692E-2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="23"/>
+        <v>0.95010289000723525</v>
+      </c>
+      <c r="Q28">
+        <f>SUM(O28:P28)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="29" spans="6:17">
+      <c r="F29">
+        <f t="shared" si="16"/>
+        <v>0.3</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="18"/>
+        <v>1.5960564314373834E-3</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="19"/>
+        <v>4.828255932177216E-6</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="22"/>
+        <v>0.99698400767383777</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="23"/>
+        <v>3.0159923261622304E-3</v>
+      </c>
+      <c r="Q29">
+        <f>SUM(O29:P29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="6:17">
+      <c r="F30">
+        <f t="shared" si="16"/>
+        <v>0.7</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="18"/>
+        <v>4.7563237850422598E-4</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="19"/>
+        <v>1.5746209193613606E-3</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="22"/>
+        <v>0.23198713007772379</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="23"/>
+        <v>0.76801286992227624</v>
+      </c>
+      <c r="Q30">
+        <f>SUM(O30:P30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="6:17">
+      <c r="I32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="6:17">
+      <c r="I33">
+        <f>SUMPRODUCT(F26:F30,O26:O30)/SUMPRODUCT(O26:O30,$S$8:$S$12)</f>
+        <v>0.39752543805421325</v>
+      </c>
+      <c r="J33">
+        <f>SUMPRODUCT(F26:F30,P26:P30)/SUMPRODUCT(P26:P30,$S$8:$S$12)</f>
+        <v>0.80510964839784094</v>
+      </c>
+    </row>
+    <row r="34" spans="6:17">
+      <c r="G34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" t="s">
+        <v>6</v>
+      </c>
+      <c r="M34" t="s">
+        <v>5</v>
+      </c>
+      <c r="O34" t="s">
+        <v>6</v>
+      </c>
+      <c r="P34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="6:17">
+      <c r="F35">
+        <f>G35/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <f>$H$5-G35</f>
+        <v>6</v>
+      </c>
+      <c r="I35">
+        <f>$I$24^G35*(1-$I$24)^H35</f>
+        <v>1.1792449762298371E-3</v>
+      </c>
+      <c r="J35">
+        <f>$J$24^G35*(1-$J$24)^H35</f>
+        <v>2.0518079881527509E-5</v>
+      </c>
+      <c r="L35">
+        <f>IF(I35&gt;J35,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <f>IF(J35&gt;I35,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f>I35/SUM($I35:$J35)</f>
+        <v>0.98289822329749832</v>
+      </c>
+      <c r="P35">
+        <f>J35/SUM($I35:$J35)</f>
+        <v>1.7101776702501643E-2</v>
+      </c>
+      <c r="Q35">
+        <f>SUM(O35:P35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="6:17">
+      <c r="F36">
+        <f t="shared" ref="F36:F39" si="24">G36/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="G36">
+        <v>9</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36:H39" si="25">$H$5-G36</f>
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ref="I36:I39" si="26">$I$24^G36*(1-$I$24)^H36</f>
+        <v>2.5964681272762835E-4</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36:J39" si="27">$J$24^G36*(1-$J$24)^H36</f>
+        <v>2.8436024776346859E-2</v>
+      </c>
+      <c r="L36">
+        <f t="shared" ref="L36:L39" si="28">IF(I36&gt;J36,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f t="shared" ref="M36:M39" si="29">IF(J36&gt;I36,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ref="O36:O39" si="30">I36/SUM($I36:$J36)</f>
+        <v>9.0482918973217412E-3</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ref="P36:P39" si="31">J36/SUM($I36:$J36)</f>
+        <v>0.9909517081026783</v>
+      </c>
+      <c r="Q36">
+        <f>SUM(O36:P36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:17">
+      <c r="F37">
+        <f t="shared" si="24"/>
+        <v>0.8</v>
+      </c>
+      <c r="G37">
+        <v>8</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="26"/>
+        <v>3.5142059004657537E-4</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="27"/>
+        <v>6.6914841011776844E-3</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="30"/>
+        <v>4.9897109992764692E-2</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="31"/>
+        <v>0.95010289000723525</v>
+      </c>
+      <c r="Q37">
+        <f>SUM(O37:P37)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="38" spans="6:17">
+      <c r="F38">
+        <f t="shared" si="24"/>
+        <v>0.3</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="25"/>
+        <v>7</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="26"/>
+        <v>1.5960564314373834E-3</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="27"/>
+        <v>4.828255932177216E-6</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="30"/>
+        <v>0.99698400767383777</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="31"/>
+        <v>3.0159923261622304E-3</v>
+      </c>
+      <c r="Q38">
+        <f>SUM(O38:P38)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:17">
+      <c r="F39">
+        <f t="shared" si="24"/>
+        <v>0.7</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="26"/>
+        <v>4.7563237850422598E-4</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="27"/>
+        <v>1.5746209193613606E-3</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="30"/>
+        <v>0.23198713007772379</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="31"/>
+        <v>0.76801286992227624</v>
+      </c>
+      <c r="Q39">
+        <f>SUM(O39:P39)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:17">
+      <c r="I41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:17">
+      <c r="I42">
+        <f>SUMPRODUCT(F35:F39,O35:O39)/SUMPRODUCT(O35:O39,$S$8:$S$12)</f>
+        <v>0.39752543805421325</v>
+      </c>
+      <c r="J42">
+        <f>SUMPRODUCT(F35:F39,P35:P39)/SUMPRODUCT(P35:P39,$S$8:$S$12)</f>
+        <v>0.80510964839784094</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -847,67 +2400,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F5:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:17">
       <c r="G5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>10</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="6:17">
+      <c r="I6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="O6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="6:17">
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="I6" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.82</v>
-      </c>
-      <c r="O6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L7" t="s">
         <v>6</v>
       </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" t="s">
-        <v>9</v>
-      </c>
       <c r="M7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="6:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="6:17">
       <c r="F8">
         <f>G8/10</f>
         <v>0.4</v>
@@ -948,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:17">
       <c r="F9">
         <f t="shared" ref="F9:F12" si="0">G9/10</f>
         <v>0.9</v>
@@ -989,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:17">
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0.8</v>
@@ -1030,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:17">
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0.3</v>
@@ -1071,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:17">
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0.7</v>
@@ -1112,15 +2665,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="I14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:17">
+      <c r="O13">
+        <f>SUM(O8:O12)</f>
+        <v>2.9209369680296442</v>
+      </c>
+    </row>
+    <row r="14" spans="6:17">
+      <c r="I14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="6:17">
       <c r="I15">
         <f>SUMPRODUCT(F8:F12,L8:L12)/SUM(L8:L12)</f>
         <v>0.46666666666666662</v>
@@ -1130,33 +2689,33 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="16" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:17">
       <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" t="s">
         <v>5</v>
       </c>
-      <c r="H16" t="s">
+      <c r="L16" t="s">
         <v>6</v>
       </c>
-      <c r="I16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" t="s">
-        <v>8</v>
-      </c>
-      <c r="L16" t="s">
-        <v>9</v>
-      </c>
       <c r="M16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="6:17">
       <c r="F17">
         <f>G17/10</f>
         <v>0.4</v>
@@ -1197,7 +2756,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:17">
       <c r="F18">
         <f t="shared" ref="F18:F21" si="8">G18/10</f>
         <v>0.9</v>
@@ -1238,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:17">
       <c r="F19">
         <f t="shared" si="8"/>
         <v>0.8</v>
@@ -1279,7 +2838,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:17">
       <c r="F20">
         <f t="shared" si="8"/>
         <v>0.3</v>
@@ -1320,7 +2879,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="21" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:17">
       <c r="F21">
         <f t="shared" si="8"/>
         <v>0.7</v>
@@ -1361,15 +2920,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="I23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:17">
+      <c r="I23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="6:17">
       <c r="I24">
         <f>SUMPRODUCT(F17:F21,L17:L21)/SUM(L17:L21)</f>
         <v>0.35</v>
@@ -1379,33 +2938,33 @@
         <v>0.80000000000000016</v>
       </c>
     </row>
-    <row r="25" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:17">
       <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" t="s">
         <v>5</v>
       </c>
-      <c r="H25" t="s">
+      <c r="L25" t="s">
         <v>6</v>
       </c>
-      <c r="I25" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" t="s">
-        <v>9</v>
-      </c>
       <c r="M25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="6:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17">
       <c r="F26">
         <f>G26/10</f>
         <v>0.4</v>
@@ -1446,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:17">
       <c r="F27">
         <f t="shared" ref="F27:F30" si="16">G27/10</f>
         <v>0.9</v>
@@ -1487,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:17">
       <c r="F28">
         <f t="shared" si="16"/>
         <v>0.8</v>
@@ -1528,7 +3087,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="29" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:17">
       <c r="F29">
         <f t="shared" si="16"/>
         <v>0.3</v>
@@ -1569,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:17">
       <c r="F30">
         <f t="shared" si="16"/>
         <v>0.7</v>
@@ -1610,15 +3169,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="I32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:17">
+      <c r="I32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="9:10">
       <c r="I33">
         <f>SUMPRODUCT(F26:F30,L26:L30)/SUM(L26:L30)</f>
         <v>0.35</v>
@@ -1632,4 +3191,989 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="55.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="45.75">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <f>9/2</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f>3/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <f>(E10-$E$7)^2+(F10-$F$7)^2</f>
+        <v>6.25</v>
+      </c>
+      <c r="I10">
+        <f>(E10-$E$8)^2+(F10-$F$8)^2</f>
+        <v>45.25</v>
+      </c>
+      <c r="J10">
+        <f>(E10-$E$9)^2+(F10-$F$9)^2</f>
+        <v>65</v>
+      </c>
+      <c r="L10">
+        <f>1/H10/(1/$H10+1/$I10+1/$J10)</f>
+        <v>0.81019196005853489</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:N10" si="0">1/I10/(1/$H10+1/$I10+1/$J10)</f>
+        <v>0.11190496685891366</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>7.7903073082551441E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H17" si="1">(E11-$E$7)^2+(F11-$F$7)^2</f>
+        <v>6.25</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I17" si="2">(E11-$E$8)^2+(F11-$F$8)^2</f>
+        <v>27.25</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11:J17" si="3">(E11-$E$9)^2+(F11-$F$9)^2</f>
+        <v>68</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L17" si="4">1/H11/(1/$H11+1/$I11+1/$J11)</f>
+        <v>0.75684782886171598</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11:M17" si="5">1/I11/(1/$H11+1/$I11+1/$J11)</f>
+        <v>0.17358895157378806</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11:N17" si="6">1/J11/(1/$H11+1/$I11+1/$J11)</f>
+        <v>6.9563219564495946E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3</v>
+      </c>
+      <c r="F12" s="6">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>15.25</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>0.97737360614918256</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>1.6022518133593157E-2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="6"/>
+        <v>6.6038757172242066E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="D13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>21.25</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>0.60176991150442483</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="5"/>
+        <v>0.17699115044247787</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="6"/>
+        <v>0.22123893805309736</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="D14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="6">
+        <v>5</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>10.25</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>0.1040582726326743</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>0.85327783558792925</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="6"/>
+        <v>4.2663891779396459E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="D15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="6">
+        <v>7</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>28.25</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>3.9980009995002494E-2</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="5"/>
+        <v>0.90354822588705641</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="6"/>
+        <v>5.6471764117941026E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="D16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="6">
+        <v>8</v>
+      </c>
+      <c r="F16" s="6">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>31.25</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>34.25</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>0.12251285490722111</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="5"/>
+        <v>0.11178180192264699</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="6"/>
+        <v>0.76570534317013195</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="6">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>51.25</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>18.25</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>7.1132764920828248E-2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="5"/>
+        <v>0.19975639464068207</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="6"/>
+        <v>0.72911084043848962</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14">
+      <c r="F20">
+        <f>SQRT(H10)</f>
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20">
+        <v>0.5</v>
+      </c>
+      <c r="M20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14">
+      <c r="H21">
+        <f>EXP(-1*$K$20*SQRT(H10))</f>
+        <v>0.28650479686019009</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:J21" si="7">EXP(-1*$K$20*SQRT(I10))</f>
+        <v>3.4617151495853357E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="7"/>
+        <v>1.7754276293213148E-2</v>
+      </c>
+      <c r="L21">
+        <f>H21/SUM($H21:$J21)</f>
+        <v>0.8454555853150455</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ref="M21:N21" si="8">I21/SUM($H21:$J21)</f>
+        <v>0.10215278906533727</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="8"/>
+        <v>5.2391625619617209E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="H22">
+        <f t="shared" ref="H22:J22" si="9">EXP(-1*$K$20*SQRT(H11))</f>
+        <v>0.28650479686019009</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>7.3528909230714978E-2</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
+        <v>1.6194143319162562E-2</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ref="L22:L28" si="10">H22/SUM($H22:$J22)</f>
+        <v>0.76151937531853375</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ref="M22:M28" si="11">I22/SUM($H22:$J22)</f>
+        <v>0.19543717815151029</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ref="N22:N28" si="12">J22/SUM($H22:$J22)</f>
+        <v>4.3043446529955939E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="H23">
+        <f t="shared" ref="H23:J23" si="13">EXP(-1*$K$20*SQRT(H12))</f>
+        <v>0.77880078307140488</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="13"/>
+        <v>0.14190997249203025</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="13"/>
+        <v>4.7768862439361105E-2</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="10"/>
+        <v>0.80414782985051558</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="11"/>
+        <v>0.14652861026097561</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="12"/>
+        <v>4.9323559888508867E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14">
+      <c r="H24">
+        <f t="shared" ref="H24:J24" si="14">EXP(-1*$K$20*SQRT(H13))</f>
+        <v>0.28650479686019009</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="14"/>
+        <v>9.9770162399103413E-2</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="14"/>
+        <v>0.12725621131859366</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="10"/>
+        <v>0.5579112102149133</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="11"/>
+        <v>0.1942825832496789</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="12"/>
+        <v>0.24780620653540786</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="H25">
+        <f t="shared" ref="H25:J25" si="15">EXP(-1*$K$20*SQRT(H14))</f>
+        <v>0.20173888639771587</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="15"/>
+        <v>0.57177084164178738</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="15"/>
+        <v>8.20849986238988E-2</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="10"/>
+        <v>0.23578790297650068</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="11"/>
+        <v>0.66827298465424823</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="12"/>
+        <v>9.5939112369251081E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14">
+      <c r="H26">
+        <f t="shared" ref="H26:J26" si="16">EXP(-1*$K$20*SQRT(H15))</f>
+        <v>7.0120754898133825E-2</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="16"/>
+        <v>0.57177084164178738</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="16"/>
+        <v>0.10687792566038574</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="10"/>
+        <v>9.3647982214980538E-2</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="11"/>
+        <v>0.7636139355159679</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="12"/>
+        <v>0.14273808226905141</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14">
+      <c r="H27">
+        <f t="shared" ref="H27:J27" si="17">EXP(-1*$K$20*SQRT(H16))</f>
+        <v>6.110968150776714E-2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="17"/>
+        <v>5.3601674127029479E-2</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="17"/>
+        <v>0.32692189535175792</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="10"/>
+        <v>0.1383720120060154</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="11"/>
+        <v>0.12137146378197274</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="12"/>
+        <v>0.74025652421201182</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14">
+      <c r="H28">
+        <f t="shared" ref="H28:J28" si="18">EXP(-1*$K$20*SQRT(H17))</f>
+        <v>2.7890887237506743E-2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="18"/>
+        <v>0.11812629428367949</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="18"/>
+        <v>0.32692189535175792</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="10"/>
+        <v>5.8973530844438293E-2</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="11"/>
+        <v>0.24977063655793941</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="12"/>
+        <v>0.69125583259762235</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14">
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14">
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <f>SUMPRODUCT(E10:E17,L$21:L$28)/SUM(L$21:L$28)</f>
+        <v>2.9578682018300064</v>
+      </c>
+      <c r="F30">
+        <f>SUMPRODUCT(F10:F17,L$21:L$28)/SUM(L$21:L$28)</f>
+        <v>4.4716601897117023</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14">
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <f>SUMPRODUCT(E10:E17,M$21:M$28)/SUM(M$21:M$28)</f>
+        <v>5.6786097626344327</v>
+      </c>
+      <c r="F31">
+        <f>SUMPRODUCT(F10:F17,M$21:M$28)/SUM(M$21:M$28)</f>
+        <v>2.7238584668390935</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14">
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <f>SUMPRODUCT(E10:E17,N$21:N$28)/SUM(N$21:N$28)</f>
+        <v>7.6576782569494339</v>
+      </c>
+      <c r="F32">
+        <f>SUMPRODUCT(F10:F17,N$21:N$28)/SUM(N$21:N$28)</f>
+        <v>4.7110751979820602</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H8:J8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>-2.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
+        <v>0.5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>-3</v>
+      </c>
+      <c r="D5">
+        <f>SQRT((B5-$B$3)^2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <f>SQRT((B5-$B$4)^2)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G5">
+        <f>EXP(-1*$J$3*D5)</f>
+        <v>0.77880078307140488</v>
+      </c>
+      <c r="H5">
+        <f>EXP(-1*$J$3*E5)</f>
+        <v>6.392786120670757E-2</v>
+      </c>
+      <c r="L5">
+        <f>G5/SUM($G5:$H5)</f>
+        <v>0.92414181997875644</v>
+      </c>
+      <c r="M5">
+        <f>H5/SUM($G5:$H5)</f>
+        <v>7.5858180021243546E-2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D11" si="0">SQRT((B6-$B$3)^2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E11" si="1">SQRT((B6-$B$4)^2)</f>
+        <v>4.5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G11" si="2">EXP(-1*$J$3*D6)</f>
+        <v>0.77880078307140488</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H12" si="3">EXP(-1*$J$3*E6)</f>
+        <v>0.10539922456186433</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L11" si="4">G6/SUM($G6:$H6)</f>
+        <v>0.88079707797788243</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M11" si="5">H6/SUM($G6:$H6)</f>
+        <v>0.11920292202211755</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0.47236655274101469</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>0.17377394345044514</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>0.73105857863000479</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>0.2689414213699951</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0.28650479686019009</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>0.28650479686019009</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0.17377394345044514</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>0.47236655274101469</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>0.2689414213699951</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>0.73105857863000479</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.10539922456186433</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>0.77880078307140488</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>0.11920292202211755</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>0.88079707797788243</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>6.392786120670757E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>0.77880078307140488</v>
+      </c>
+      <c r="L11">
+        <f>G11/SUM($G11:$H11)</f>
+        <v>7.5858180021243546E-2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>0.92414181997875644</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="L14">
+        <f>SUMPRODUCT(B5:B11,L5:L11)/SUMPRODUCT(L5:L11,O5:O11)</f>
+        <v>-1.2943303968697368</v>
+      </c>
+      <c r="M14">
+        <f>SUMPRODUCT(B5:B11,M5:M11)/SUMPRODUCT(M5:M11,O5:O11)</f>
+        <v>1.2943303968697368</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>